<commit_message>
calcolo rivisto arrotondamento mulitplo qli trasporti
</commit_message>
<xml_diff>
--- a/arrotondamento peso.xlsx
+++ b/arrotondamento peso.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Lubex\GESLUX\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBDC4987-FD7F-4A63-98E6-68065CD48A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{3803D6B8-A11A-44FD-9F5B-6C9A8EBD96EA}"/>
+    <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -184,7 +178,7 @@
         <xdr:cNvPr id="2" name="Immagine 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A36CE37-CB43-EA3C-5069-F4F8D8CEF957}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8A36CE37-CB43-EA3C-5069-F4F8D8CEF957}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -256,7 +250,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -308,7 +302,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -502,23 +496,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C831969-1DE0-4DEA-AB11-0D6BC41B9C14}">
-  <dimension ref="A1:N7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,8 +543,24 @@
         <v>265</v>
       </c>
       <c r="N1" s="2"/>
+      <c r="O1" s="1">
+        <v>250</v>
+      </c>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="1">
+        <v>280</v>
+      </c>
+      <c r="R1" s="2"/>
+      <c r="S1" s="1">
+        <v>290</v>
+      </c>
+      <c r="T1" s="2"/>
+      <c r="U1" s="1">
+        <v>191.56</v>
+      </c>
+      <c r="V1" s="2"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -583,8 +593,24 @@
         <v>2.6</v>
       </c>
       <c r="N2" s="4"/>
+      <c r="O2" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="R2" s="4"/>
+      <c r="S2" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="T2" s="4"/>
+      <c r="U2" s="3">
+        <v>1.9156</v>
+      </c>
+      <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="3"/>
@@ -599,8 +625,16 @@
       <c r="L3" s="4"/>
       <c r="M3" s="3"/>
       <c r="N3" s="4"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="4"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -644,8 +678,32 @@
       <c r="N4" s="4">
         <v>3</v>
       </c>
+      <c r="O4" s="3">
+        <v>1</v>
+      </c>
+      <c r="P4" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>1</v>
+      </c>
+      <c r="R4" s="4">
+        <v>3</v>
+      </c>
+      <c r="S4" s="3">
+        <v>1</v>
+      </c>
+      <c r="T4" s="4">
+        <v>3</v>
+      </c>
+      <c r="U4" s="3">
+        <v>1</v>
+      </c>
+      <c r="V4" s="4">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0.5</v>
       </c>
@@ -688,8 +746,32 @@
       <c r="N5" s="4">
         <v>3</v>
       </c>
+      <c r="O5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="P5" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="R5" s="4">
+        <v>3</v>
+      </c>
+      <c r="S5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="T5" s="4">
+        <v>3</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="V5" s="4">
+        <v>2</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>0.2</v>
       </c>
@@ -732,8 +814,32 @@
       <c r="N6" s="4">
         <v>2.8</v>
       </c>
+      <c r="O6" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="P6" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="R6" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="T6" s="4">
+        <v>3</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V6" s="4">
+        <v>2</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>0.1</v>
       </c>
@@ -775,6 +881,30 @@
       </c>
       <c r="N7" s="6">
         <v>2.7</v>
+      </c>
+      <c r="O7" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="P7" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="R7" s="6">
+        <v>2.8</v>
+      </c>
+      <c r="S7" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="T7" s="6">
+        <v>2.9</v>
+      </c>
+      <c r="U7" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="V7" s="6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -785,23 +915,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6d90398c-565e-42bf-b860-3cabf23a8727" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010050E46C3D20B98243B62E6A58C16C2818" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="45596db27ec581463a17bd43ad3c9559">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="778c9873-604f-4b89-a96d-7a3132ee6aa4" xmlns:ns4="6d90398c-565e-42bf-b860-3cabf23a8727" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1f85508f7fac79d53e0799c18949dd46" ns3:_="" ns4:_="">
     <xsd:import namespace="778c9873-604f-4b89-a96d-7a3132ee6aa4"/>
@@ -1016,32 +1129,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3E1037C-93E8-454E-96DB-5C3DA2C7CCBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="778c9873-604f-4b89-a96d-7a3132ee6aa4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="6d90398c-565e-42bf-b860-3cabf23a8727"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0536548B-08AA-4273-BBCE-26B2CB6EC534}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6d90398c-565e-42bf-b860-3cabf23a8727" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E30B6112-4FB3-49B5-9E47-46855639FCAE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1058,4 +1163,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0536548B-08AA-4273-BBCE-26B2CB6EC534}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3E1037C-93E8-454E-96DB-5C3DA2C7CCBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="778c9873-604f-4b89-a96d-7a3132ee6aa4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="6d90398c-565e-42bf-b860-3cabf23a8727"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>